<commit_message>
Entries 1.23.2020 and 1.25.2020
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CAF221-126F-45D4-834B-9393060D4AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101D584A-C498-4173-9BCA-CBE0B7D8157F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -118,6 +118,39 @@
   </si>
   <si>
     <t>This exercise helped boost my confidence in being able to read and understand code on my own. As someone who is generally not confidant in their own abilities, I hope that there are future exercises that help boost my confidance in similar fashion. While many of the courses I have taken in the past felt very theory based, this class feels very practical and I would highly recommend others to take similar classes (not that they exist at the moment!)</t>
+  </si>
+  <si>
+    <t>Nic</t>
+  </si>
+  <si>
+    <t>Search for certain functions, and write down thought process and priority.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was able to locate and identify potential findings and solutioins to our problem. </t>
+  </si>
+  <si>
+    <t>The activity allowed us to be very purposeful and reflective for our every move. It forced us to really slow down and think about what decisions we were making, and make a usually thoughtless process to become very meaningful.</t>
+  </si>
+  <si>
+    <t>To be very honest this activity felt….very slow, and I questioned whether or not it would be useful in the future. The first minute into the activity felt meaningful, but it quickly felt like a manual task that took more time trying to find reasons to my actions than getting the task at hand done.</t>
+  </si>
+  <si>
+    <t>3:00 - 7:00</t>
+  </si>
+  <si>
+    <t>Nic, Rafael, Chris</t>
+  </si>
+  <si>
+    <t>Finding 2 features to look for in FreeCol and creating a UML document.</t>
+  </si>
+  <si>
+    <t>We were able to successfully identify 2 features we wanted to look for, find them within the program, and create a uml documentation of the entire project.</t>
+  </si>
+  <si>
+    <t>There was so much code! Luckily the code was not as hard to sift through, thanks to the project being well documented. But after having created the UML document, the code base seemed so vast and big that it made me think that perhaps we had almost gotten lucky in terms of how relatively quickly we got through the initial process.</t>
+  </si>
+  <si>
+    <t>Even though we had a few struggles, I realized very quickly how in comparison to some other programs, FreeCol is probably quite small in size. This made me appreciate people's ability to actually "read" code. Even with nice documentation, it may still be very hard to find or understand certain programs...so imagine a program that has poor to no documentation! just thinking about it gives me chills.</t>
   </si>
 </sst>
 </file>
@@ -262,7 +295,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,11 +331,14 @@
     <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -624,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,24 +670,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -792,7 +828,7 @@
       <c r="A12" s="11">
         <v>43848</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <v>0.41666666666666669</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -811,23 +847,51 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+    <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>43853</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
+        <v>43855</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
updating 1.28.2020 in case of no save
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101D584A-C498-4173-9BCA-CBE0B7D8157F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB448A3B-6A33-4E97-A146-42F0FD1D70E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -660,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Diary entries 2.1.2020 and 1.30.2020
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB448A3B-6A33-4E97-A146-42F0FD1D70E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C35D44-C5BA-4674-BF4A-BCB9A143CA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -151,6 +151,42 @@
   </si>
   <si>
     <t>Even though we had a few struggles, I realized very quickly how in comparison to some other programs, FreeCol is probably quite small in size. This made me appreciate people's ability to actually "read" code. Even with nice documentation, it may still be very hard to find or understand certain programs...so imagine a program that has poor to no documentation! just thinking about it gives me chills.</t>
+  </si>
+  <si>
+    <t>2.1.2020</t>
+  </si>
+  <si>
+    <t>1:00 - 5:00</t>
+  </si>
+  <si>
+    <t>Finding 2 essential features for our program, and write a packet for others to be able to follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accomplished all set out goals. </t>
+  </si>
+  <si>
+    <t>1.30.2020</t>
+  </si>
+  <si>
+    <t>5:00 - 8:00</t>
+  </si>
+  <si>
+    <t>Learning different notations for UML documentation</t>
+  </si>
+  <si>
+    <t>Scraped the surface and quickly went over some tools to generate UML and other relational diagrams.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I realized I was often times making those relational diagrams when trying to communicate to others what my code should look like or require. </t>
+  </si>
+  <si>
+    <t>Learning about it made me want to learn other forms of communication. I wondered if UML is the single most used form of graphical form of code was.</t>
+  </si>
+  <si>
+    <t>As we looked for "essential" features from our game, we quickly realized that what may not be essential to run the program can still considered essential to the game logic. Thus, although in parallel programs our features may not be essential to their code, we felt that in our specific cases our features were essential.</t>
+  </si>
+  <si>
+    <t>Overall I felt pretty accomplished and good about the amount of work we were able to do in the given time. Now that we've gone through the code numerous times, it felt much easier to sift through the code and identify the important features.</t>
   </si>
 </sst>
 </file>
@@ -295,7 +331,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,20 +361,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -660,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="57" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,24 +709,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -779,137 +818,165 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>43839</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="14">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="12">
         <v>43846</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="12">
         <v>43848</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="16">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="12">
         <v>43853</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15">
+    <row r="14" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
         <v>43855</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
+    <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>

</xml_diff>

<commit_message>
Updating diary entries up to 2.19.2020 (#340)
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C35D44-C5BA-4674-BF4A-BCB9A143CA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E74696-E55B-42C1-9346-0755647BE153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -187,6 +187,93 @@
   </si>
   <si>
     <t>Overall I felt pretty accomplished and good about the amount of work we were able to do in the given time. Now that we've gone through the code numerous times, it felt much easier to sift through the code and identify the important features.</t>
+  </si>
+  <si>
+    <t>2.6.2020</t>
+  </si>
+  <si>
+    <t>Briefly Talk about Exam + Guest speaker</t>
+  </si>
+  <si>
+    <t>Learned what it means to be a developer in a smaller company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It made me really think about what it would be like to work at a small company as opposed to some place like Blizzard. It's very cool to see how much creative freedom someone in that position can have. </t>
+  </si>
+  <si>
+    <t>I felt small, thinking that there are so many options and choices we can make even under the same umbrella of "software engineer". I'm not quite sure if I would necessaryily like it better, but it's definitely something to think about.</t>
+  </si>
+  <si>
+    <t>2.13.2020</t>
+  </si>
+  <si>
+    <t>Exam day</t>
+  </si>
+  <si>
+    <t>Finished the exam! Whoot whoot. Also learned about  different stakeholders and what impact they may have on software development.</t>
+  </si>
+  <si>
+    <t>I've never really thought much about stakeholders other than the developer and the person who provides the requirements. It made me really think about, for example, in game development, how much the players really contribute to the game development, along with the investors who can really stear the direction of development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really hope that the people who invest in my work could give me a sense of creative freedom….I am not particularly fond of people who restrict me and throw money at me saying they get to decide…but then again it probably is how the world realistically works. </t>
+  </si>
+  <si>
+    <t>2.15.2020</t>
+  </si>
+  <si>
+    <t>2:00 - 7:00</t>
+  </si>
+  <si>
+    <t>Find Essential Feature (re-do)</t>
+  </si>
+  <si>
+    <t>Found our 2nd re-do essential feature (map generation). Wrote out outline of what we would write once we confirm with Kaj</t>
+  </si>
+  <si>
+    <t>We feel like we have a much clearer understanding as a group as to what an essential feature actually is. Before we considered what users may REALLY want, but that's different from a core part of the code that may break if it does not exist in the program</t>
+  </si>
+  <si>
+    <t>While it was initially frustrating to see how poorly we did on the assignment, it was refreshing to feel like we fully understood the concepts now, and hopefully don't run into such problems in the future.</t>
+  </si>
+  <si>
+    <t>2.18.2020</t>
+  </si>
+  <si>
+    <t>Nic, Rafael, Chris, Kaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with Kaj </t>
+  </si>
+  <si>
+    <t>3:45 - 4:30</t>
+  </si>
+  <si>
+    <t>Going over resubmission</t>
+  </si>
+  <si>
+    <t>It seems like we were on the right track, and we just needed to refine our writing and thought process. We also were going too low-level, and made it hard for the reader to really understand things at a high-level.</t>
+  </si>
+  <si>
+    <t>It felt good to be reassured that we weren't completely off the right track. It seems like Kaj is grading us….not harshly, but very realistically, which probably most people aren't used to. Even at an academic/university level. I hope that this version of our resubmission is much easier to understand.</t>
+  </si>
+  <si>
+    <t>2.19.2020</t>
+  </si>
+  <si>
+    <t>2:30 - 5:00</t>
+  </si>
+  <si>
+    <t>Complete Resubmission</t>
+  </si>
+  <si>
+    <t>Finished rewriting our first essential feature to be more legible and redid 2nd feature entirely.</t>
+  </si>
+  <si>
+    <t>It was good that we ended up meeting as a group rather than working independently. We regrouped every 10 minutes to make sure we were all on the same page, and rubber-duckied back and forth with what we planned on doing.</t>
+  </si>
+  <si>
+    <t>I feel great with our new submission. It feels complete, much more legible than our pervious iteration, and showcases a much higher-level understanding of the code rather than a lower-level repeat of code.</t>
   </si>
 </sst>
 </file>
@@ -331,7 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,9 +448,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -378,6 +462,12 @@
     </xf>
     <xf numFmtId="18" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -699,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="57" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,24 +799,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -818,516 +908,586 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="11">
         <v>43839</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>43846</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="11">
         <v>43848</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="11">
         <v>43853</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="11">
         <v>43855</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="78" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="156" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+    <row r="17" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="17"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="17"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="17"/>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="17"/>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="17"/>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="17"/>
     </row>
     <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="17"/>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="17"/>
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="17"/>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="17"/>
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="17"/>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>

</xml_diff>

<commit_message>
Diary entry up to 3.3.2020
</commit_message>
<xml_diff>
--- a/diaries/diary-HyunYang.xlsx
+++ b/diaries/diary-HyunYang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyun\IdeaProjects\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E74696-E55B-42C1-9346-0755647BE153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD6538C-A371-4642-ABB4-0E1C8E22C3BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -274,6 +274,78 @@
   </si>
   <si>
     <t>I feel great with our new submission. It feels complete, much more legible than our pervious iteration, and showcases a much higher-level understanding of the code rather than a lower-level repeat of code.</t>
+  </si>
+  <si>
+    <t>2.20.2020</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Architectual Understanding</t>
+  </si>
+  <si>
+    <t>Being able to understand that Architectual design of a program</t>
+  </si>
+  <si>
+    <t>It was an extremely tough process for me. Realizing that I wasn't trying to identify how the program should be architect, but the fact that we had to identify how the program is architected as is made the activity much more challening.</t>
+  </si>
+  <si>
+    <t>After seeing that the homework was to come up with the architectual model of our open-source program, I dreaded it. It felt daunting to me that I struggled so much with PacMan, and now to do that with our huge project, it seemed near impossible to do. I am not sure how to even approach things.</t>
+  </si>
+  <si>
+    <t>2.21.2020</t>
+  </si>
+  <si>
+    <t>2:00 - 7:30</t>
+  </si>
+  <si>
+    <t>Architectual Model of Open Source</t>
+  </si>
+  <si>
+    <t>We were able to generate the architectual model and find issues/pull requests that were interesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The assignment was actual not as hard as I had envisioned, unlike how I felt the day before. Once we abstracted most of the functionality of the program, it was a lot easier to see the overall architectual model. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I personally enjoyed finding some of the issues that people ran into, and it was cool </t>
+  </si>
+  <si>
+    <t>2.27.2020</t>
+  </si>
+  <si>
+    <t>5:00 - 8:00 pm</t>
+  </si>
+  <si>
+    <t>Architectual Patterns</t>
+  </si>
+  <si>
+    <t>Learned about forms of architectual practices / patterns that are well built common coding practices that has knowledge built on them for common coding problems</t>
+  </si>
+  <si>
+    <t>The class tied very closely with Professor Malek's Architecture course, and drew a lot of knowledge we knew from that class to this topic.</t>
+  </si>
+  <si>
+    <t>Actually utilizing something we learned in one class and applying it to better our knowledge of how other systems worked felt very useful. While it's hard for me to truly grasp what some architectual patterns are, it probably will become more clear to me as I continue to grow and become more exposed to future coding challenges.</t>
+  </si>
+  <si>
+    <t>3.1.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:00 - 7:00 pm </t>
+  </si>
+  <si>
+    <t>Identifying Architectual Patterns in Code, Solve issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was able to identify and solve an issue within FreeCol, and find a couple of the architectual patterns. </t>
+  </si>
+  <si>
+    <t>Started by trying to find the easiest bug to fix. Given our current understanding of the game, it would be both extremely hard to identify and test a bug that is embedded in the gaming logic. We decide to look for bugs that were centered around the map editor, as that is something we had access to as soon as we open the game. Not only did we get to tackle an issue others seem to be having, but getting a thumbs up for our bug fix felt very reassuring and ultimately felt great!</t>
+  </si>
+  <si>
+    <t>Given how small our bug was, it seems crazy to think how long it might take others to solve certain issues / bugs that are exponentially larger in scale. It also feels a little daunting to try and tackle a second issue. I can imagine how hard it must be for others with much more complicated projects probably struggle a lot more than us.</t>
   </si>
 </sst>
 </file>
@@ -463,11 +535,11 @@
     <xf numFmtId="18" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -789,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="57" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,24 +871,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1078,7 +1150,7 @@
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1087,7 +1159,7 @@
       <c r="F17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1183,41 +1255,97 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="17"/>
+    <row r="22" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="234" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
@@ -1226,7 +1354,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
@@ -1235,7 +1363,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="17"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
@@ -1244,7 +1372,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
@@ -1253,7 +1381,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
@@ -1262,7 +1390,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="17"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
@@ -1271,7 +1399,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
@@ -1280,7 +1408,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
@@ -1289,7 +1417,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="17"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
@@ -1298,7 +1426,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="17"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
@@ -1307,7 +1435,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="17"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
@@ -1316,7 +1444,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="17"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
@@ -1325,7 +1453,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="17"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
@@ -1334,7 +1462,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="17"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
@@ -1343,7 +1471,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="17"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
@@ -1352,7 +1480,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="17"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
@@ -1361,7 +1489,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="17"/>
+      <c r="G41" s="16"/>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
@@ -1370,7 +1498,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
@@ -1379,7 +1507,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="17"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
@@ -1388,7 +1516,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
@@ -1397,7 +1525,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="17"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
@@ -1406,7 +1534,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="17"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
@@ -1415,7 +1543,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
@@ -1424,7 +1552,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="17"/>
+      <c r="G48" s="16"/>
     </row>
     <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
@@ -1433,7 +1561,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="17"/>
+      <c r="G49" s="16"/>
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
@@ -1442,7 +1570,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="17"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
@@ -1451,7 +1579,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="17"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
@@ -1460,7 +1588,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="17"/>
+      <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
@@ -1469,7 +1597,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="17"/>
+      <c r="G53" s="16"/>
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
@@ -1478,7 +1606,7 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
@@ -1487,7 +1615,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="17"/>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>

</xml_diff>